<commit_message>
add filter export based on unit
</commit_message>
<xml_diff>
--- a/directory/templates/template-absensi.xlsx
+++ b/directory/templates/template-absensi.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hrmis-master\directory\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19425768-F4EA-4D75-BEB2-E5EDDFB2178F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661B34DB-4ED2-4400-BFDF-FE014CB91159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{31A0B364-D528-4097-98D0-DBAC8A79801F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>NO</t>
   </si>
@@ -36,18 +36,9 @@
     <t>TANGGAL</t>
   </si>
   <si>
-    <t>Export Date : {app_export_date}</t>
-  </si>
-  <si>
-    <t>[pegawai_nama]</t>
-  </si>
-  <si>
     <t>NAMA PEGAWAI</t>
   </si>
   <si>
-    <t>SIMABSEN | ABSEN {status}</t>
-  </si>
-  <si>
     <t>[tanggal_absen]</t>
   </si>
   <si>
@@ -84,27 +75,9 @@
     <t>[verifikasi_m]</t>
   </si>
   <si>
-    <t>[mesin_m]</t>
-  </si>
-  <si>
     <t>[verifikasi_p]</t>
   </si>
   <si>
-    <t>[mesin_p]</t>
-  </si>
-  <si>
-    <t>ID ABSEN</t>
-  </si>
-  <si>
-    <t>[absen_id]</t>
-  </si>
-  <si>
-    <t>User : {user}</t>
-  </si>
-  <si>
-    <t>[jam_kerja] Jam</t>
-  </si>
-  <si>
     <t>SHIFT</t>
   </si>
   <si>
@@ -121,6 +94,27 @@
   </si>
   <si>
     <t>[nama_sub_unit]</t>
+  </si>
+  <si>
+    <t>[nama]</t>
+  </si>
+  <si>
+    <t>[mesin_masuk]</t>
+  </si>
+  <si>
+    <t>[mesin_pulang]</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>: {cxfilter_unit}</t>
+  </si>
+  <si>
+    <t>SIMABSEN | ABSEN PERIODE {status}</t>
+  </si>
+  <si>
+    <t>[jam_kerja]</t>
   </si>
 </sst>
 </file>
@@ -130,7 +124,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;Rp&quot;* #,##0_-;&quot;-Rp&quot;* #,##0_-;_-&quot;Rp&quot;* \-_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,13 +172,6 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -328,7 +315,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -388,20 +375,22 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -419,9 +408,21 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -743,49 +744,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6F3688-F949-4382-8B45-577625C51054}">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="7.6640625" customWidth="1"/>
     <col min="3" max="3" width="23.44140625" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.21875" customWidth="1"/>
     <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
+      <c r="B1" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
       <c r="T1" s="7"/>
@@ -798,22 +797,22 @@
     </row>
     <row r="2" spans="1:26" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
       <c r="R2" s="7"/>
       <c r="S2" s="7"/>
       <c r="T2" s="7"/>
@@ -854,10 +853,12 @@
     </row>
     <row r="4" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="3"/>
+      <c r="B4" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>27</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -883,9 +884,7 @@
     </row>
     <row r="5" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
       <c r="E5" s="3"/>
@@ -938,43 +937,41 @@
     </row>
     <row r="7" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="32"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="32"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="32"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="M7" s="32"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="P7" s="26" t="s">
-        <v>26</v>
-      </c>
+      <c r="O7" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="14"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
@@ -988,33 +985,33 @@
     </row>
     <row r="8" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
-      <c r="H8" s="34"/>
+      <c r="H8" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="I8" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="N8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
+        <v>14</v>
+      </c>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="14"/>
       <c r="Q8" s="21"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
@@ -1032,48 +1029,46 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>4</v>
-      </c>
       <c r="F9" s="6" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>13</v>
+        <v>22</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="J9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="O9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="O9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q9" s="25"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="24"/>
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
       <c r="T9" s="11"/>
@@ -1085,7 +1080,7 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -1098,8 +1093,8 @@
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
       <c r="P10" s="22"/>
       <c r="Q10" s="22"/>
       <c r="R10" s="13"/>
@@ -1113,23 +1108,33 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
     </row>
+    <row r="18" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="35"/>
+    </row>
+    <row r="19" spans="8:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="35"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H20" s="36"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="P7:P8"/>
+  <mergeCells count="11">
+    <mergeCell ref="O7:O8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:N8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="H7:H8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="B1:Q2"/>
+    <mergeCell ref="B1:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>